<commit_message>
Arregladas funciones de timeit y actualizado excel a tiempos verdaderos
</commit_message>
<xml_diff>
--- a/Analisis de Sorting Algorithms.xlsx
+++ b/Analisis de Sorting Algorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Analisis de Algoritmos\tarea_3_analisis_de_algoritmos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9C6574-6C9A-4D51-B6ED-97E57210DC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3508D8-3F3F-4860-9326-9E4CE6F8C478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12708" yWindow="7476" windowWidth="10332" windowHeight="4764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>Insertion Sort</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Quick Sort</t>
   </si>
   <si>
-    <t>Arreglo de tamaño pequeño (7 elementos)</t>
-  </si>
-  <si>
     <t>Test 1</t>
   </si>
   <si>
@@ -112,6 +109,15 @@
   </si>
   <si>
     <t>Arreglo de tamaño muy grande (10,000 elementos)</t>
+  </si>
+  <si>
+    <t>Arreglo de tamaño mediano (1000 elementos)</t>
+  </si>
+  <si>
+    <t>x10^-5</t>
+  </si>
+  <si>
+    <t>Arreglo de tamaño pequeño (10 elementos)</t>
   </si>
 </sst>
 </file>
@@ -161,21 +167,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -205,7 +220,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64BFF103-5955-4144-90BE-88097447C1E0}" name="Tabla3" displayName="Tabla3" ref="B3:H19" totalsRowShown="0">
   <autoFilter ref="B3:H19" xr:uid="{64BFF103-5955-4144-90BE-88097447C1E0}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{03009FFA-3F0D-40F3-8B2E-440E70EF6D3E}" name="Tests" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{03009FFA-3F0D-40F3-8B2E-440E70EF6D3E}" name="Tests" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{B5E7BE10-1CE2-429E-B170-BC91BE617E72}" name="Insertion Sort"/>
     <tableColumn id="3" xr3:uid="{5FB51663-FE00-4A1C-85B7-B5493A7FCB6C}" name="Selection Sort"/>
     <tableColumn id="4" xr3:uid="{45B1D9CC-35EF-4451-8A7C-4FE8F763A5D2}" name="Bubble Sort"/>
@@ -218,16 +233,32 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1C964A59-78A8-4B4B-A01C-1EEA968C2657}" name="Tabla35" displayName="Tabla35" ref="B22:H38" totalsRowShown="0">
-  <autoFilter ref="B22:H38" xr:uid="{1C964A59-78A8-4B4B-A01C-1EEA968C2657}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1C964A59-78A8-4B4B-A01C-1EEA968C2657}" name="Tabla35" displayName="Tabla35" ref="B23:H39" totalsRowShown="0">
+  <autoFilter ref="B23:H39" xr:uid="{1C964A59-78A8-4B4B-A01C-1EEA968C2657}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2497E640-8C13-4C6D-9584-6CB82E7B294E}" name="Tests" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2497E640-8C13-4C6D-9584-6CB82E7B294E}" name="Tests" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{7DF08914-C061-4643-85ED-E5109E27909F}" name="Insertion Sort"/>
     <tableColumn id="3" xr3:uid="{D269807E-E229-4DF2-9819-64A3B281B7E0}" name="Selection Sort"/>
     <tableColumn id="4" xr3:uid="{1BBD3C22-E5F2-49D9-953A-EDFC44B7A266}" name="Bubble Sort"/>
     <tableColumn id="5" xr3:uid="{DB9D423F-F16F-4866-AB23-50D466CBF605}" name="Merge Sort"/>
     <tableColumn id="6" xr3:uid="{65CD15DD-06C0-4C88-A274-2C9D8D13F2B7}" name="Heap Sort"/>
     <tableColumn id="7" xr3:uid="{169798CE-BB2D-4A8D-BE41-CF3491A4C005}" name="Quick Sort"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B7A1AAC-722E-40B3-A9B9-FF44D999BF0D}" name="Tabla32" displayName="Tabla32" ref="J3:P19" totalsRowShown="0">
+  <autoFilter ref="J3:P19" xr:uid="{1B7A1AAC-722E-40B3-A9B9-FF44D999BF0D}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F046030E-76E8-4B27-97FF-C8D7C793DBD7}" name="Tests" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E600D2BD-56AF-4F80-A14C-6FB01BDAAD80}" name="Insertion Sort"/>
+    <tableColumn id="3" xr3:uid="{D35205ED-19E2-4693-BE17-3824BCE9F1AC}" name="Selection Sort"/>
+    <tableColumn id="4" xr3:uid="{B488C6C1-443C-4709-88FC-A50C6EDF6CAC}" name="Bubble Sort"/>
+    <tableColumn id="5" xr3:uid="{A4D50358-4D0A-4A67-9A7D-93788725DDD0}" name="Merge Sort"/>
+    <tableColumn id="6" xr3:uid="{E5FB862F-BB7C-4589-AF59-D1F5FE1D06A2}" name="Heap Sort"/>
+    <tableColumn id="7" xr3:uid="{DA5E83D3-A2AD-4B38-954E-9B513F36A629}" name="Quick Sort"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -496,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H38"/>
+  <dimension ref="B2:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,17 +547,23 @@
     <col min="18" max="18" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -546,143 +583,256 @@
       <c r="H3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>1.1000019999999999</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>3.3114299993030699E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>4.4806999503634801E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="C5">
+        <v>1.0700019999999999</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>3.3790000015869702E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>3.1092999852262398E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="C6">
+        <v>0.8999952</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>3.2341599988285397E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>3.94119997508823E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="C7">
+        <v>0.93999549999999998</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>3.9883799967355998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>3.0420999974012301E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="C8">
+        <v>1.0200009999999999</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>3.27010999899357E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
-        <v>3.5948999575339201E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="C9">
+        <v>0.89000089999999998</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>3.2112799992319099E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>3.7878000293858302E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="C10">
+        <v>1.0700019999999999</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <v>3.3216499956324697E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
-        <v>2.9779999749734898E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3">
+        <v>1.0500020000000001</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="J11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3.4716999973170397E-2</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4">
-        <v>5.5608000257052403E-3</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="C12">
+        <v>1.84999</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12">
+        <v>3.34590999991633E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
-        <v>3.91500000841915E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="C13">
+        <v>1.0400020000000001</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13">
+        <v>4.0326900023501297E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
-        <v>3.7252999609336201E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="C14">
+        <v>0.91000099999999995</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>3.3037300046999001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14">
-        <v>3.5183000145480002E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+      <c r="C15">
+        <v>1.06999</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15">
+        <v>3.2226499984972103E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15">
-        <v>2.9444000101648202E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+      <c r="C16">
+        <v>0.99000100000000002</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16">
+        <v>3.3075399987865198E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
-        <v>3.1428000074811202E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+      <c r="C17">
+        <v>1.0500020000000001</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17">
+        <v>3.4407400002237402E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17">
-        <v>3.9566999766975598E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C18">
-        <v>4.5340000069700103E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>0.93000099999999997</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18">
+        <v>3.2712799962609999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C19">
         <f>AVERAGE(C4:C18)</f>
-        <v>3.7487533253927961E-3</v>
+        <v>1.05866584</v>
       </c>
       <c r="D19" t="e">
         <f>AVERAGE(D4:D18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E19" t="e">
-        <f t="shared" ref="D19:H19" si="0">AVERAGE(E4:E18)</f>
+        <f t="shared" ref="E19:H19" si="0">AVERAGE(E4:E18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F19" t="e">
@@ -697,200 +847,237 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="J19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
+      <c r="K19">
+        <f>AVERAGE(K4:K18)</f>
+        <v>3.4074833325576002E-2</v>
+      </c>
+      <c r="L19" t="e">
+        <f>AVERAGE(L4:L18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" t="e">
+        <f t="shared" ref="M19" si="1">AVERAGE(M4:M18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" t="e">
+        <f>AVERAGE(N4:N18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" t="e">
+        <f t="shared" ref="O19:P19" si="2">AVERAGE(O4:O18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
         <v>0</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>2</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>3</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>4</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>3.5558737000101202</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C23">
-        <v>80.58</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
+      <c r="C25">
+        <v>3.5857949999626699</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C24">
-        <v>91.85</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
+      <c r="C26">
+        <v>3.6907640999997899</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C25">
-        <v>82.38</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
+      <c r="C27">
+        <v>3.7333265999914098</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C26">
-        <v>81.12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
+      <c r="C28">
+        <v>3.6413443000055801</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27">
-        <v>82.11</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
+      <c r="C29">
+        <v>3.6359979000408198</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C28">
-        <v>80.16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
+      <c r="C30">
+        <v>3.6565957999555301</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C29">
-        <v>79.33</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
+      <c r="C31" s="3">
+        <v>3.5369630999630299</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="4">
-        <v>78.430000000000007</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
+      <c r="C32">
+        <v>3.5786460000090301</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C31">
-        <v>79.7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
+      <c r="C33">
+        <v>3.5345999000128301</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C32">
-        <v>79.569999999999993</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="3" t="s">
+      <c r="C34">
+        <v>3.5232586000347501</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C33">
-        <v>81.150000000000006</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
+      <c r="C35">
+        <v>3.5870397999533399</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C34">
-        <v>81.62</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="3" t="s">
+      <c r="C36">
+        <v>3.5964906000299299</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C35">
-        <v>79.680000000000007</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="3" t="s">
+      <c r="C37">
+        <v>3.5905539999948801</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C36">
-        <v>81.61</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37">
-        <v>81.34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="C38">
-        <f>AVERAGE(C23:C37)</f>
-        <v>81.37533333333333</v>
-      </c>
-      <c r="D38" t="e">
-        <f>AVERAGE(D23:D37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E38" t="e">
-        <f t="shared" ref="E38" si="1">AVERAGE(E23:E37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F38" t="e">
-        <f>AVERAGE(F23:F37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G38" t="e">
-        <f t="shared" ref="G38" si="2">AVERAGE(G23:G37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H38" t="e">
-        <f t="shared" ref="H38" si="3">AVERAGE(H23:H37)</f>
+        <v>3.5899874999886299</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39">
+        <f>AVERAGE(C24:C38)</f>
+        <v>3.6024824599968226</v>
+      </c>
+      <c r="D39" t="e">
+        <f>AVERAGE(D24:D38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E39" t="e">
+        <f t="shared" ref="E39" si="3">AVERAGE(E24:E38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F39" t="e">
+        <f>AVERAGE(F24:F38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G39" t="e">
+        <f t="shared" ref="G39" si="4">AVERAGE(G24:G38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" t="e">
+        <f t="shared" ref="H39" si="5">AVERAGE(H24:H38)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>